<commit_message>
Fixed bug on validation
</commit_message>
<xml_diff>
--- a/ViventiumCompaniesEmployeesDataStore/DATA2.xlsx
+++ b/ViventiumCompaniesEmployeesDataStore/DATA2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\source\repos\ViventiumCompaniesEmployeesDataStore\ViventiumCompaniesEmployeesDataStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F584BB-7B4C-4DF0-9C65-394BAC616157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB5EA9-1C9C-4021-8B1A-26760CEBB7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391B1D1A-B96A-439D-9FD6-8317BFA71698}"/>
   </bookViews>
@@ -12769,8 +12769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568C6753-232A-4B9D-B184-22F966D5B631}">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A985" workbookViewId="0">
-      <selection activeCell="H1006" sqref="H1006"/>
+    <sheetView tabSelected="1" topLeftCell="A979" workbookViewId="0">
+      <selection activeCell="A1003" sqref="A1003:XFD1003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>